<commit_message>
Upload latest plots and codes that correspond to the paper
</commit_message>
<xml_diff>
--- a/code/out/Fig4/repeat/results.xlsx
+++ b/code/out/Fig4/repeat/results.xlsx
@@ -14454,13 +14454,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.301437754092957</v>
+        <v>0.3014377541465457</v>
       </c>
       <c r="C2">
-        <v>0.2718629232727579</v>
+        <v>0.271619767310625</v>
       </c>
       <c r="D2">
-        <v>0.3407657157402922</v>
+        <v>0.3406654197030673</v>
       </c>
     </row>
   </sheetData>
@@ -14623,10 +14623,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C2">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D2">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -14637,10 +14637,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C3">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D3">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -14651,10 +14651,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C4">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D4">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -14665,10 +14665,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C5">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D5">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -14679,10 +14679,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C6">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D6">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -14693,10 +14693,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C7">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D7">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -14707,10 +14707,10 @@
         <v>0.7341310425527023</v>
       </c>
       <c r="C8">
-        <v>0.65136281997312</v>
+        <v>0.6515511293757743</v>
       </c>
       <c r="D8">
-        <v>0.8109021762520572</v>
+        <v>0.8108782692900148</v>
       </c>
     </row>
   </sheetData>
@@ -14745,13 +14745,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.006380667098853721</v>
+        <v>0.006380667099988056</v>
       </c>
       <c r="C2">
-        <v>0.004277940222099923</v>
+        <v>0.004277940215035393</v>
       </c>
       <c r="D2">
-        <v>0.008181540000420292</v>
+        <v>0.008181540003611472</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -14759,13 +14759,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.03066265384790661</v>
+        <v>0.03066265385310671</v>
       </c>
       <c r="C3">
-        <v>0.02604743094695337</v>
+        <v>0.02604743092587195</v>
       </c>
       <c r="D3">
-        <v>0.03412693047005977</v>
+        <v>0.03412693046904088</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -14773,13 +14773,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.07366851818526389</v>
+        <v>0.07366851819695869</v>
       </c>
       <c r="C4">
-        <v>0.07043468974725091</v>
+        <v>0.0704346895532072</v>
       </c>
       <c r="D4">
-        <v>0.07660970553197691</v>
+        <v>0.07660970982023857</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -14787,13 +14787,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1318662084262431</v>
+        <v>0.1318662084456961</v>
       </c>
       <c r="C5">
-        <v>0.1291098925496024</v>
+        <v>0.1291098924506222</v>
       </c>
       <c r="D5">
-        <v>0.134707700170143</v>
+        <v>0.1347076942122074</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -14801,13 +14801,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.19481717560941</v>
+        <v>0.1948171756357494</v>
       </c>
       <c r="C6">
-        <v>0.1915262469181262</v>
+        <v>0.1915262472575975</v>
       </c>
       <c r="D6">
-        <v>0.1982346307076276</v>
+        <v>0.1982346306505026</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -14815,13 +14815,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.2510661033668338</v>
+        <v>0.2510661033973442</v>
       </c>
       <c r="C7">
-        <v>0.2471168759349189</v>
+        <v>0.2471168760653517</v>
       </c>
       <c r="D7">
-        <v>0.2551612196740077</v>
+        <v>0.2551612266184433</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -14829,13 +14829,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.2974334585602058</v>
+        <v>0.2974334585922074</v>
       </c>
       <c r="C8">
-        <v>0.2928087167625798</v>
+        <v>0.2928087161327464</v>
       </c>
       <c r="D8">
-        <v>0.3016884989614249</v>
+        <v>0.3016884993128832</v>
       </c>
     </row>
   </sheetData>

</xml_diff>